<commit_message>
modified:   app/Http/Controllers/Administrasi.php 	modified:   app/Imports/ImportExcelPayroll.php 	modified:   public/file_excel/ContohUploadPayroll.xlsx 	deleted:    public/file_excel/Periode-2404_upload-20240426testupload.xlsx 	deleted:    public/file_excel/Periode-2404_upload-20240518Contoh Format Upload Tambahan dan Potongan Payroll (1).xlsx 	new file:   public/file_excel/c_payroll/Periode-2405_upload-20240614-Contoh Format Upload Tambahan dan Potongan Payroll (1).xlsx 	new file:   public/file_excel/c_payroll/Periode-2406_upload-20240613Contoh Format Upload Tambahan dan Potongan Payroll (1).xlsx 	modified:   resources/views/products/04_administrasi/bpjs.blade.php 	modified:   resources/views/products/04_administrasi/payroll.blade.php 	new file:   resources/views/products/04_administrasi/tambahanPayroll.blade.php 	modified:   routes/web.php
</commit_message>
<xml_diff>
--- a/public/file_excel/ContohUploadPayroll.xlsx
+++ b/public/file_excel/ContohUploadPayroll.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laravel\Kerjaan\pintex-ehrd\public\file_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D82365-0A1D-45F6-8332-646BD04BF54A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395FE1AE-CFEC-45F2-8698-D2382874BB1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{A61AD1BD-B57A-4C16-B979-A5F8443ECAFC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="12780" xr2:uid="{A61AD1BD-B57A-4C16-B979-A5F8443ECAFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,33 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>STB</t>
   </si>
   <si>
     <t>NAMA</t>
-  </si>
-  <si>
-    <t>JENIS</t>
-  </si>
-  <si>
-    <t>NOMINAL</t>
-  </si>
-  <si>
-    <t>PERIODE</t>
-  </si>
-  <si>
-    <t>PRESTASI</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>JABATAN</t>
-  </si>
-  <si>
-    <t>ABSEN</t>
   </si>
   <si>
     <t>KOPERASI</t>
@@ -69,10 +48,7 @@
     <t>PINJAMAN</t>
   </si>
   <si>
-    <t>SELISIH</t>
-  </si>
-  <si>
-    <t>JENIS :</t>
+    <t>PERIODE</t>
   </si>
 </sst>
 </file>
@@ -81,9 +57,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +83,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -151,16 +133,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -476,204 +465,226 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6E7DD97-8182-408F-BF41-951422F4B3FD}">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="str">
+        <f ca="1">RIGHT(YEAR(TODAY()),2)&amp;TEXT(TODAY(),"mm")</f>
+        <v>2406</v>
+      </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="3"/>
       <c r="E2" s="2"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="str">
+        <f t="shared" ref="A3:A20" ca="1" si="0">RIGHT(YEAR(TODAY()),2)&amp;TEXT(TODAY(),"mm")</f>
+        <v>2406</v>
+      </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="3"/>
       <c r="E3" s="2"/>
-      <c r="K3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+    </row>
+    <row r="4" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>2406</v>
+      </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="3"/>
       <c r="E4" s="2"/>
-      <c r="K4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>2406</v>
+      </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="3"/>
       <c r="E5" s="2"/>
-      <c r="K5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>2406</v>
+      </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="3"/>
       <c r="E6" s="2"/>
-      <c r="K6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>2406</v>
+      </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="3"/>
       <c r="E7" s="2"/>
-      <c r="K7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>2406</v>
+      </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="3"/>
       <c r="E8" s="2"/>
-      <c r="K8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>2406</v>
+      </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="3"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>2406</v>
+      </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="3"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>2406</v>
+      </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="3"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>2406</v>
+      </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="3"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>2406</v>
+      </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="3"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>2406</v>
+      </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="3"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>2406</v>
+      </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="3"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>2406</v>
+      </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="3"/>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
+      <c r="A17" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>2406</v>
+      </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="3"/>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
+      <c r="A18" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>2406</v>
+      </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="3"/>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
+      <c r="A19" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>2406</v>
+      </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="3"/>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
+      <c r="A20" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>2406</v>
+      </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="3"/>

</xml_diff>